<commit_message>
updated controller towards spec
</commit_message>
<xml_diff>
--- a/Cars Endpoint Spec.xlsx
+++ b/Cars Endpoint Spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anguyen/Onedrive Swinburne/OneDrive - Swinburne University/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/103681990_student_swin_edu_au/Documents/Documents/IOO/Cars-2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A38ACF1-14B8-2649-9008-54561526BB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{8A38ACF1-14B8-2649-9008-54561526BB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9F54783-32B2-4E77-9C33-1E45ED2A3550}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="-19260" windowWidth="40960" windowHeight="22540" xr2:uid="{82FBC1DB-F515-DB43-AB57-CFE322635606}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82FBC1DB-F515-DB43-AB57-CFE322635606}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Endpoint Url</t>
   </si>
@@ -96,13 +96,22 @@
     <t>Add a new car</t>
   </si>
   <si>
-    <t>Updates a car given a car in the body</t>
-  </si>
-  <si>
     <t>Returns a car given a rego as a parameter</t>
   </si>
   <si>
     <t>Delete a car given a rego as a parameter</t>
+  </si>
+  <si>
+    <t>Updates a car given a car in the body, based on matched rego</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Rego</t>
   </si>
 </sst>
 </file>
@@ -501,20 +510,20 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="16.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.375" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="41.125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -534,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="148" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -550,19 +559,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="107" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="107.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -580,26 +591,40 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+    <row r="6" spans="1:6" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>